<commit_message>
changes to support multiple sequences
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,15 +436,20 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>start</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>end</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>probability</t>
         </is>
@@ -454,98 +459,38 @@
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B2" t="n">
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>NC_002620.2</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
         <v>1</v>
       </c>
-      <c r="C2" t="n">
-        <v>89000</v>
-      </c>
       <c r="D2" t="n">
-        <v>0.9999940528911688</v>
+        <v>39000</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.9591354048217994</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B3" t="n">
-        <v>100001</v>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>NC_000964.3</t>
+        </is>
       </c>
       <c r="C3" t="n">
-        <v>135000</v>
+        <v>1</v>
       </c>
       <c r="D3" t="n">
-        <v>0.9937928382123643</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="n">
-        <v>145001</v>
-      </c>
-      <c r="C4" t="n">
-        <v>160000</v>
-      </c>
-      <c r="D4" t="n">
-        <v>0.9633040125692653</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="n">
-        <v>180001</v>
-      </c>
-      <c r="C5" t="n">
-        <v>630000</v>
-      </c>
-      <c r="D5" t="n">
-        <v>0.9833769910975004</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="n">
-        <v>640001</v>
-      </c>
-      <c r="C6" t="n">
-        <v>938000</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0.9875595725641136</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="n">
-        <v>951001</v>
-      </c>
-      <c r="C7" t="n">
-        <v>3785000</v>
-      </c>
-      <c r="D7" t="n">
-        <v>0.9999934822048562</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="n">
-        <v>3785001</v>
-      </c>
-      <c r="C8" t="n">
-        <v>4220000</v>
-      </c>
-      <c r="D8" t="n">
-        <v>0.9838800176692748</v>
+        <v>30000</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.9999930385485697</v>
       </c>
     </row>
   </sheetData>

</xml_diff>